<commit_message>
Added Nearest Fault Line Names
</commit_message>
<xml_diff>
--- a/data/cleaned/Fault Line Distance Data.xlsx
+++ b/data/cleaned/Fault Line Distance Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adriandm.lazaro/Documents/GitHub/Site-Selection-Project/data/cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE69B7C-A3D1-744E-874E-81F900898426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51783672-E17C-3C4E-9A2E-90CDC87FBDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="77">
   <si>
     <t>Region</t>
   </si>
@@ -229,6 +229,33 @@
   </si>
   <si>
     <t>Tarlac</t>
+  </si>
+  <si>
+    <t>Nearest Fault Line Name</t>
+  </si>
+  <si>
+    <t>Valley Fault System</t>
+  </si>
+  <si>
+    <t>Lubang Fault</t>
+  </si>
+  <si>
+    <t>Philippine Fault</t>
+  </si>
+  <si>
+    <t>Unnamed Fault</t>
+  </si>
+  <si>
+    <t>Iba Fault</t>
+  </si>
+  <si>
+    <t>Nagtipunan Fault</t>
+  </si>
+  <si>
+    <t>Casiguran Fault</t>
+  </si>
+  <si>
+    <t>Care Fault</t>
   </si>
 </sst>
 </file>
@@ -277,13 +304,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,27 +527,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="26" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -534,6 +564,9 @@
       <c r="C2" s="2">
         <v>9.4</v>
       </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -545,6 +578,9 @@
       <c r="C3" s="2">
         <v>3.7</v>
       </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -556,6 +592,9 @@
       <c r="C4" s="2">
         <v>2.2999999999999998</v>
       </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -567,6 +606,9 @@
       <c r="C5" s="2">
         <v>11</v>
       </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -578,6 +620,9 @@
       <c r="C6" s="2">
         <v>1.9</v>
       </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -590,6 +635,9 @@
       <c r="C7" s="1">
         <v>5.4</v>
       </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -601,6 +649,9 @@
       <c r="C8" s="2">
         <v>0</v>
       </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -612,6 +663,9 @@
       <c r="C9" s="2">
         <v>0</v>
       </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -623,6 +677,9 @@
       <c r="C10" s="2">
         <v>12.2</v>
       </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -634,6 +691,9 @@
       <c r="C11" s="2">
         <v>1.2</v>
       </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -645,6 +705,9 @@
       <c r="C12" s="2">
         <v>3.7</v>
       </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -656,6 +719,9 @@
       <c r="C13" s="2">
         <v>0</v>
       </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -664,8 +730,11 @@
       <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>0.48699999999999999</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -678,6 +747,9 @@
       <c r="C15" s="1">
         <v>0</v>
       </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -689,8 +761,11 @@
       <c r="C16" s="2">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -700,8 +775,11 @@
       <c r="C17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -711,8 +789,11 @@
       <c r="C18" s="2">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -722,8 +803,11 @@
       <c r="C19" s="2">
         <v>27.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -733,8 +817,11 @@
       <c r="C20" s="2">
         <v>61.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -744,8 +831,11 @@
       <c r="C21" s="1">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -755,8 +845,11 @@
       <c r="C22" s="2">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -766,8 +859,11 @@
       <c r="C23" s="2">
         <v>22.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -777,19 +873,25 @@
       <c r="C24" s="1">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -799,30 +901,39 @@
       <c r="C26" s="2">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -832,8 +943,11 @@
       <c r="C29" s="2">
         <v>30.6</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
@@ -843,41 +957,53 @@
       <c r="C30" s="2">
         <v>12.3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32">
         <v>34.799999999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
@@ -887,8 +1013,11 @@
       <c r="C34" s="2">
         <v>37.200000000000003</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
@@ -898,8 +1027,11 @@
       <c r="C35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>21</v>
       </c>
@@ -909,8 +1041,11 @@
       <c r="C36" s="2">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -920,8 +1055,11 @@
       <c r="C37" s="2">
         <v>19.8</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>21</v>
       </c>
@@ -931,8 +1069,11 @@
       <c r="C38" s="2">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
@@ -942,8 +1083,11 @@
       <c r="C39" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -953,8 +1097,11 @@
       <c r="C40" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -964,8 +1111,11 @@
       <c r="C41" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -975,8 +1125,11 @@
       <c r="C42" s="1">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -986,8 +1139,11 @@
       <c r="C43" s="2">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
@@ -997,8 +1153,11 @@
       <c r="C44" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>39</v>
       </c>
@@ -1008,8 +1167,11 @@
       <c r="C45" s="2">
         <v>26.9</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
@@ -1019,8 +1181,11 @@
       <c r="C46" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>39</v>
       </c>
@@ -1030,8 +1195,11 @@
       <c r="C47" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>39</v>
       </c>
@@ -1041,8 +1209,11 @@
       <c r="C48" s="1">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>39</v>
       </c>
@@ -1052,8 +1223,11 @@
       <c r="C49" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>39</v>
       </c>
@@ -1063,8 +1237,11 @@
       <c r="C50" s="2">
         <v>13.1</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>39</v>
       </c>
@@ -1074,8 +1251,11 @@
       <c r="C51" s="2">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>39</v>
       </c>
@@ -1085,8 +1265,11 @@
       <c r="C52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>39</v>
       </c>
@@ -1096,8 +1279,11 @@
       <c r="C53" s="2">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>39</v>
       </c>
@@ -1107,8 +1293,11 @@
       <c r="C54" s="2">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>39</v>
       </c>
@@ -1118,8 +1307,11 @@
       <c r="C55" s="2">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>39</v>
       </c>
@@ -1129,8 +1321,11 @@
       <c r="C56" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>39</v>
       </c>
@@ -1140,8 +1335,11 @@
       <c r="C57" s="2">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>39</v>
       </c>
@@ -1151,8 +1349,11 @@
       <c r="C58" s="2">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>39</v>
       </c>
@@ -1162,8 +1363,11 @@
       <c r="C59" s="2">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>39</v>
       </c>
@@ -1173,8 +1377,11 @@
       <c r="C60" s="1">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>39</v>
       </c>
@@ -1184,8 +1391,11 @@
       <c r="C61" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>39</v>
       </c>
@@ -1195,8 +1405,11 @@
       <c r="C62" s="2">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>39</v>
       </c>
@@ -1206,8 +1419,11 @@
       <c r="C63" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D63" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>